<commit_message>
Updates to code and source files
</commit_message>
<xml_diff>
--- a/CO_County_Sales_2014_2018.xlsx
+++ b/CO_County_Sales_2014_2018.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\Colorado Marijuana Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davem\OneDrive\Documents\GitHub\CO-Marijuana-Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8959AA0F-91F9-4A49-B2AA-5CDF66E8DADD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{8959AA0F-91F9-4A49-B2AA-5CDF66E8DADD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{8FDCA1D0-464B-419C-AF0C-B112D063A73E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CO Sales 2014-2018 - OLD" sheetId="1" state="hidden" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2763" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2763" uniqueCount="156">
   <si>
     <t>Link_to_Original_File</t>
   </si>
@@ -509,6 +509,9 @@
   </si>
   <si>
     <t>NW</t>
+  </si>
+  <si>
+    <t>Not Reported</t>
   </si>
 </sst>
 </file>
@@ -9781,7 +9784,7 @@
   <dimension ref="A1:K326"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="B66" sqref="B66:B326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11930,7 +11933,7 @@
         <v>146</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="F66" s="9">
         <v>2014</v>
@@ -14056,8 +14059,8 @@
       <c r="A131" t="s">
         <v>146</v>
       </c>
-      <c r="B131" t="s">
-        <v>147</v>
+      <c r="B131" s="6" t="s">
+        <v>155</v>
       </c>
       <c r="C131" s="2"/>
       <c r="D131" s="2"/>
@@ -16173,7 +16176,7 @@
         <v>146</v>
       </c>
       <c r="B196" s="6" t="s">
-        <v>61</v>
+        <v>155</v>
       </c>
       <c r="F196" s="11">
         <v>2016</v>
@@ -18329,8 +18332,8 @@
       <c r="A261" t="s">
         <v>146</v>
       </c>
-      <c r="B261" t="s">
-        <v>61</v>
+      <c r="B261" s="6" t="s">
+        <v>155</v>
       </c>
       <c r="C261" s="2"/>
       <c r="D261" s="2"/>
@@ -20464,7 +20467,7 @@
         <v>146</v>
       </c>
       <c r="B326" s="6" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="F326" s="11">
         <v>2018</v>

</xml_diff>

<commit_message>
Updated excel files and CCMDs RMD file
In the excel files, blank entries in the sales/tax columns were changed to "NR" to reflect how the state of Colorado is reporting those values.

The rmd file was updated to pull the excel files from github and perform initial cleaning.
</commit_message>
<xml_diff>
--- a/CO_County_Sales_2014_2018.xlsx
+++ b/CO_County_Sales_2014_2018.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davem\OneDrive\Documents\GitHub\CO-Marijuana-Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{8959AA0F-91F9-4A49-B2AA-5CDF66E8DADD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{8FDCA1D0-464B-419C-AF0C-B112D063A73E}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{8959AA0F-91F9-4A49-B2AA-5CDF66E8DADD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{7AB8A8C9-DBE6-4086-8379-51F19EC753FD}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'2016 County Sales'!$A$1:$XFC$67</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'2017 County Sales'!$A$1:$K$67</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'2018 County Sales'!$A$1:$K$67</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">aggregate!$A$1:$K$326</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">aggregate!$A$1:$K$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CO Sales 2014-2018 - OLD'!$A$1:$J$305</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2763" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2995" uniqueCount="156">
   <si>
     <t>Link_to_Original_File</t>
   </si>
@@ -9784,7 +9784,7 @@
   <dimension ref="A1:K326"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66:B326"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9895,8 +9895,14 @@
       <c r="G3" s="10">
         <v>15758</v>
       </c>
+      <c r="H3" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I3" s="10">
         <v>0</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="K3" s="10">
         <v>0</v>
@@ -9959,6 +9965,18 @@
       <c r="G5" s="10">
         <v>12240</v>
       </c>
+      <c r="H5" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
@@ -10125,9 +10143,15 @@
       <c r="H10" s="10">
         <v>438167</v>
       </c>
+      <c r="I10" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="J10" s="10">
         <v>23.745027908741125</v>
       </c>
+      <c r="K10" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -10256,6 +10280,18 @@
       <c r="G14" s="10">
         <v>3563</v>
       </c>
+      <c r="H14" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
@@ -10562,9 +10598,15 @@
       <c r="H23" s="10">
         <v>67026306</v>
       </c>
+      <c r="I23" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="J23" s="10">
         <v>101.02797979630503</v>
       </c>
+      <c r="K23" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
@@ -10693,6 +10735,18 @@
       <c r="G27" s="10">
         <v>14535</v>
       </c>
+      <c r="H27" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="K27" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
@@ -10964,8 +11018,14 @@
       <c r="H35" s="10">
         <v>0</v>
       </c>
+      <c r="I35" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="J35" s="10">
         <v>0</v>
+      </c>
+      <c r="K35" s="10" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -11165,8 +11225,14 @@
       <c r="G41" s="10">
         <v>147735</v>
       </c>
+      <c r="H41" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I41" s="10">
         <v>0</v>
+      </c>
+      <c r="J41" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="K41" s="10">
         <v>0</v>
@@ -11229,8 +11295,14 @@
       <c r="G43" s="10">
         <v>12944</v>
       </c>
+      <c r="H43" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I43" s="10">
         <v>0</v>
+      </c>
+      <c r="J43" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="K43" s="10">
         <v>0</v>
@@ -11261,9 +11333,15 @@
       <c r="H44" s="10">
         <v>1045651</v>
       </c>
+      <c r="I44" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="J44" s="10">
         <v>41.063894125039269</v>
       </c>
+      <c r="K44" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
@@ -11287,8 +11365,14 @@
       <c r="G45" s="10">
         <v>40564</v>
       </c>
+      <c r="H45" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I45" s="10">
         <v>0</v>
+      </c>
+      <c r="J45" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="K45" s="10">
         <v>0</v>
@@ -11316,6 +11400,18 @@
       <c r="G46" s="10">
         <v>28007</v>
       </c>
+      <c r="H46" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="I46" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="J46" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="K46" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
@@ -11374,6 +11470,18 @@
       <c r="G48" s="10">
         <v>4560</v>
       </c>
+      <c r="H48" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="I48" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="J48" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="K48" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
@@ -11397,6 +11505,18 @@
       <c r="G49" s="10">
         <v>16353</v>
       </c>
+      <c r="H49" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="I49" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="J49" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="K49" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
@@ -11665,6 +11785,18 @@
       <c r="G57" s="10">
         <v>6199</v>
       </c>
+      <c r="H57" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="I57" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="J57" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="K57" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
@@ -11758,6 +11890,18 @@
       <c r="G60" s="10">
         <v>2327</v>
       </c>
+      <c r="H60" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="I60" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="J60" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="K60" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
@@ -11816,8 +11960,14 @@
       <c r="G62" s="10">
         <v>23406</v>
       </c>
+      <c r="H62" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I62" s="10">
         <v>0</v>
+      </c>
+      <c r="J62" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="K62" s="10">
         <v>0</v>
@@ -12002,9 +12152,14 @@
       <c r="G68" s="7">
         <v>15854</v>
       </c>
-      <c r="H68" s="7"/>
+      <c r="H68" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I68" s="7">
         <v>0</v>
+      </c>
+      <c r="J68" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="K68" s="10">
         <v>0</v>
@@ -12067,8 +12222,18 @@
       <c r="G70" s="7">
         <v>12401</v>
       </c>
-      <c r="H70" s="7"/>
-      <c r="I70" s="7"/>
+      <c r="H70" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="I70" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="J70" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="K70" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
@@ -12232,10 +12397,15 @@
       <c r="G75" s="7">
         <v>18578</v>
       </c>
-      <c r="H75" s="7"/>
+      <c r="H75" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I75" s="7">
         <v>1817143</v>
       </c>
+      <c r="J75" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K75" s="10">
         <v>97.811551297233294</v>
       </c>
@@ -12335,9 +12505,14 @@
       <c r="H78" s="7">
         <v>0</v>
       </c>
-      <c r="I78" s="7"/>
+      <c r="I78" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="J78" s="10">
         <v>0</v>
+      </c>
+      <c r="K78" s="10" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
@@ -12362,8 +12537,18 @@
       <c r="G79" s="7">
         <v>3577</v>
       </c>
-      <c r="H79" s="7"/>
-      <c r="I79" s="7"/>
+      <c r="H79" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="I79" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="J79" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="K79" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
@@ -12670,10 +12855,15 @@
       <c r="H88" s="7">
         <v>86100007</v>
       </c>
-      <c r="I88" s="7"/>
+      <c r="I88" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="J88" s="10">
         <v>127.55688873810543</v>
       </c>
+      <c r="K88" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
@@ -12802,10 +12992,15 @@
       <c r="G92" s="7">
         <v>14686</v>
       </c>
-      <c r="H92" s="7"/>
+      <c r="H92" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I92" s="7">
         <v>1380296</v>
       </c>
+      <c r="J92" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K92" s="10">
         <v>93.987198692632433</v>
       </c>
@@ -12832,10 +13027,15 @@
       <c r="G93" s="7">
         <v>16120</v>
       </c>
-      <c r="H93" s="7"/>
+      <c r="H93" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I93" s="7">
         <v>3262219</v>
       </c>
+      <c r="J93" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K93" s="10">
         <v>202.37090570719602</v>
       </c>
@@ -12900,9 +13100,14 @@
       <c r="H95" s="7">
         <v>0</v>
       </c>
-      <c r="I95" s="7"/>
+      <c r="I95" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="J95" s="10">
         <v>0</v>
+      </c>
+      <c r="K95" s="10" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
@@ -13070,10 +13275,15 @@
       <c r="H100" s="10">
         <v>6725788</v>
       </c>
-      <c r="I100" s="7"/>
+      <c r="I100" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="J100" s="10">
         <v>909.01310987971351</v>
       </c>
+      <c r="K100" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
@@ -13167,10 +13377,15 @@
       <c r="G103" s="7">
         <v>14029</v>
       </c>
-      <c r="H103" s="7"/>
+      <c r="H103" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I103" s="7">
         <v>8598642</v>
       </c>
+      <c r="J103" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K103" s="10">
         <v>612.91909615795851</v>
       </c>
@@ -13267,8 +13482,18 @@
       <c r="G106" s="7">
         <v>148597</v>
       </c>
-      <c r="H106" s="7"/>
-      <c r="I106" s="7"/>
+      <c r="H106" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="I106" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="J106" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="K106" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
@@ -13327,9 +13552,14 @@
       <c r="G108" s="7">
         <v>12952</v>
       </c>
-      <c r="H108" s="7"/>
+      <c r="H108" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I108" s="7">
         <v>0</v>
+      </c>
+      <c r="J108" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="K108" s="10">
         <v>0</v>
@@ -13392,9 +13622,14 @@
       <c r="G110" s="7">
         <v>40552</v>
       </c>
-      <c r="H110" s="7"/>
+      <c r="H110" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I110" s="7">
         <v>0</v>
+      </c>
+      <c r="J110" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="K110" s="10">
         <v>0</v>
@@ -13422,8 +13657,18 @@
       <c r="G111" s="7">
         <v>28108</v>
       </c>
-      <c r="H111" s="7"/>
-      <c r="I111" s="7"/>
+      <c r="H111" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="I111" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="J111" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="K111" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
@@ -13482,10 +13727,15 @@
       <c r="G113" s="7">
         <v>4587</v>
       </c>
-      <c r="H113" s="7"/>
+      <c r="H113" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I113" s="7">
         <v>342075</v>
       </c>
+      <c r="J113" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K113" s="10">
         <v>74.574885546108561</v>
       </c>
@@ -13512,10 +13762,15 @@
       <c r="G114" s="7">
         <v>16704</v>
       </c>
-      <c r="H114" s="7"/>
+      <c r="H114" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I114" s="7">
         <v>1815654</v>
       </c>
+      <c r="J114" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K114" s="10">
         <v>108.69576149425288</v>
       </c>
@@ -13790,9 +14045,14 @@
       <c r="H122" s="7">
         <v>0</v>
       </c>
-      <c r="I122" s="7"/>
+      <c r="I122" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="J122" s="10">
         <v>0</v>
+      </c>
+      <c r="K122" s="10" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
@@ -13820,9 +14080,14 @@
       <c r="H123" s="7">
         <v>0</v>
       </c>
-      <c r="I123" s="7"/>
+      <c r="I123" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="J123" s="10">
         <v>0</v>
+      </c>
+      <c r="K123" s="10" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
@@ -13882,8 +14147,18 @@
       <c r="G125" s="7">
         <v>2371</v>
       </c>
-      <c r="H125" s="7"/>
-      <c r="I125" s="7"/>
+      <c r="H125" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="I125" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="J125" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="K125" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
@@ -13942,9 +14217,14 @@
       <c r="G127" s="7">
         <v>23351</v>
       </c>
-      <c r="H127" s="7"/>
+      <c r="H127" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I127" s="7">
         <v>0</v>
+      </c>
+      <c r="J127" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="K127" s="10">
         <v>0</v>
@@ -14132,8 +14412,14 @@
       <c r="G133" s="10">
         <v>16006</v>
       </c>
+      <c r="H133" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I133" s="10">
         <v>0</v>
+      </c>
+      <c r="J133" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="K133" s="10">
         <v>0</v>
@@ -14196,6 +14482,18 @@
       <c r="G135" s="10">
         <v>12839</v>
       </c>
+      <c r="H135" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="I135" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="J135" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="K135" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
@@ -14359,9 +14657,15 @@
       <c r="G140" s="10">
         <v>19077</v>
       </c>
+      <c r="H140" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I140" s="10">
         <v>2291010</v>
       </c>
+      <c r="J140" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K140" s="10">
         <v>120.09278188394401</v>
       </c>
@@ -14493,9 +14797,15 @@
       <c r="G144" s="10">
         <v>3700</v>
       </c>
+      <c r="H144" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I144" s="10">
         <v>2836422</v>
       </c>
+      <c r="J144" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K144" s="10">
         <v>766.60054054054058</v>
       </c>
@@ -14805,9 +15115,15 @@
       <c r="H153" s="10">
         <v>101137059</v>
       </c>
+      <c r="I153" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="J153" s="10">
         <v>146.77071669264325</v>
       </c>
+      <c r="K153" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="6" t="s">
@@ -14901,9 +15217,15 @@
       <c r="G156" s="10">
         <v>5901</v>
       </c>
+      <c r="H156" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I156" s="10">
         <v>2654538</v>
       </c>
+      <c r="J156" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K156" s="10">
         <v>449.84544992374174</v>
       </c>
@@ -14930,9 +15252,15 @@
       <c r="G157" s="10">
         <v>15124</v>
       </c>
+      <c r="H157" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I157" s="10">
         <v>3292626</v>
       </c>
+      <c r="J157" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K157" s="10">
         <v>217.70867495371596</v>
       </c>
@@ -14959,9 +15287,15 @@
       <c r="G158" s="10">
         <v>16433</v>
       </c>
+      <c r="H158" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I158" s="10">
         <v>5421591</v>
       </c>
+      <c r="J158" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K158" s="10">
         <v>329.92095174344308</v>
       </c>
@@ -15026,8 +15360,14 @@
       <c r="H160" s="10">
         <v>0</v>
       </c>
+      <c r="I160" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="J160" s="10">
         <v>0</v>
+      </c>
+      <c r="K160" s="10" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.25">
@@ -15297,9 +15637,15 @@
       <c r="G168" s="10">
         <v>14059</v>
       </c>
+      <c r="H168" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I168" s="10">
         <v>21456457</v>
       </c>
+      <c r="J168" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K168" s="10">
         <v>1526.1723451170069</v>
       </c>
@@ -15396,6 +15742,18 @@
       <c r="G171" s="10">
         <v>150258</v>
       </c>
+      <c r="H171" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="I171" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="J171" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="K171" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="6" t="s">
@@ -15454,8 +15812,14 @@
       <c r="G173" s="10">
         <v>13169</v>
       </c>
+      <c r="H173" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I173" s="10">
         <v>0</v>
+      </c>
+      <c r="J173" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="K173" s="10">
         <v>0</v>
@@ -15518,8 +15882,14 @@
       <c r="G175" s="10">
         <v>41142</v>
       </c>
+      <c r="H175" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I175" s="10">
         <v>0</v>
+      </c>
+      <c r="J175" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="K175" s="10">
         <v>0</v>
@@ -15547,9 +15917,15 @@
       <c r="G176" s="10">
         <v>28015</v>
       </c>
+      <c r="H176" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I176" s="10">
         <v>4138320</v>
       </c>
+      <c r="J176" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K176" s="10">
         <v>147.71800820988756</v>
       </c>
@@ -15576,8 +15952,14 @@
       <c r="G177" s="10">
         <v>18206</v>
       </c>
+      <c r="H177" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I177" s="10">
         <v>0</v>
+      </c>
+      <c r="J177" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="K177" s="10">
         <v>0</v>
@@ -15605,9 +15987,15 @@
       <c r="G178" s="10">
         <v>4766</v>
       </c>
+      <c r="H178" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I178" s="10">
         <v>2877032</v>
       </c>
+      <c r="J178" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K178" s="10">
         <v>603.65757448594206</v>
       </c>
@@ -15634,9 +16022,15 @@
       <c r="G179" s="10">
         <v>17339</v>
       </c>
+      <c r="H179" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I179" s="10">
         <v>3331577</v>
       </c>
+      <c r="J179" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K179" s="10">
         <v>192.14354922429206</v>
       </c>
@@ -15911,8 +16305,14 @@
       <c r="H187" s="10">
         <v>0</v>
       </c>
+      <c r="I187" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="J187" s="10">
         <v>0</v>
+      </c>
+      <c r="K187" s="10" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="188" spans="1:11" x14ac:dyDescent="0.25">
@@ -15940,8 +16340,14 @@
       <c r="H188" s="10">
         <v>0</v>
       </c>
+      <c r="I188" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="J188" s="10">
         <v>0</v>
+      </c>
+      <c r="K188" s="10" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="189" spans="1:11" x14ac:dyDescent="0.25">
@@ -16001,6 +16407,18 @@
       <c r="G190" s="10">
         <v>2399</v>
       </c>
+      <c r="H190" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="I190" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="J190" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="K190" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="6" t="s">
@@ -16059,8 +16477,14 @@
       <c r="G192" s="10">
         <v>24012</v>
       </c>
+      <c r="H192" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I192" s="10">
         <v>0</v>
+      </c>
+      <c r="J192" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="K192" s="10">
         <v>0</v>
@@ -16245,9 +16669,14 @@
       <c r="G198" s="7">
         <v>16056</v>
       </c>
-      <c r="H198" s="7"/>
+      <c r="H198" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I198" s="7">
         <v>0</v>
+      </c>
+      <c r="J198" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="K198" s="10">
         <v>0</v>
@@ -16310,10 +16739,15 @@
       <c r="G200" s="7">
         <v>13316</v>
       </c>
-      <c r="H200" s="7"/>
+      <c r="H200" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I200" s="7">
         <v>6397398</v>
       </c>
+      <c r="J200" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K200" s="10">
         <v>480.42940823069989</v>
       </c>
@@ -16480,10 +16914,15 @@
       <c r="G205" s="7">
         <v>19623</v>
       </c>
-      <c r="H205" s="7"/>
+      <c r="H205" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I205" s="7">
         <v>4014966</v>
       </c>
+      <c r="J205" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K205" s="10">
         <v>204.60510625286653</v>
       </c>
@@ -16615,10 +17054,15 @@
       <c r="G209" s="7">
         <v>3771</v>
       </c>
-      <c r="H209" s="7"/>
+      <c r="H209" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I209" s="7">
         <v>3874954</v>
       </c>
+      <c r="J209" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K209" s="10">
         <v>1027.5666931848316</v>
       </c>
@@ -16928,10 +17372,15 @@
       <c r="H218" s="7">
         <v>102115436</v>
       </c>
-      <c r="I218" s="7"/>
+      <c r="I218" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="J218" s="10">
         <v>145.61230772740819</v>
       </c>
+      <c r="K218" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
@@ -17025,10 +17474,15 @@
       <c r="G221" s="7">
         <v>6000</v>
       </c>
-      <c r="H221" s="7"/>
+      <c r="H221" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I221" s="7">
         <v>2553596</v>
       </c>
+      <c r="J221" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K221" s="10">
         <v>425.59933333333333</v>
       </c>
@@ -17055,10 +17509,15 @@
       <c r="G222" s="7">
         <v>15297</v>
       </c>
-      <c r="H222" s="7"/>
+      <c r="H222" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I222" s="7">
         <v>3957092</v>
       </c>
+      <c r="J222" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K222" s="10">
         <v>258.68418644178598</v>
       </c>
@@ -17085,10 +17544,15 @@
       <c r="G223" s="7">
         <v>16871</v>
       </c>
-      <c r="H223" s="7"/>
+      <c r="H223" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I223" s="7">
         <v>6880647</v>
       </c>
+      <c r="J223" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K223" s="10">
         <v>407.83871732558828</v>
       </c>
@@ -17153,9 +17617,14 @@
       <c r="H225" s="7">
         <v>0</v>
       </c>
-      <c r="I225" s="7"/>
+      <c r="I225" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="J225" s="10">
         <v>0</v>
+      </c>
+      <c r="K225" s="10" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="226" spans="1:11" x14ac:dyDescent="0.25">
@@ -17530,10 +17999,15 @@
       <c r="G236" s="7">
         <v>151900</v>
       </c>
-      <c r="H236" s="7"/>
+      <c r="H236" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I236" s="7">
         <v>3965609</v>
       </c>
+      <c r="J236" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K236" s="10">
         <v>26.106708360763662</v>
       </c>
@@ -17595,9 +18069,14 @@
       <c r="G238" s="7">
         <v>13112</v>
       </c>
-      <c r="H238" s="7"/>
+      <c r="H238" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I238" s="7">
         <v>0</v>
+      </c>
+      <c r="J238" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="K238" s="10">
         <v>0</v>
@@ -17660,9 +18139,14 @@
       <c r="G240" s="7">
         <v>41763</v>
       </c>
-      <c r="H240" s="7"/>
+      <c r="H240" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I240" s="7">
         <v>0</v>
+      </c>
+      <c r="J240" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="K240" s="10">
         <v>0</v>
@@ -17690,10 +18174,15 @@
       <c r="G241" s="7">
         <v>28075</v>
       </c>
-      <c r="H241" s="7"/>
+      <c r="H241" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I241" s="7">
         <v>7918706</v>
       </c>
+      <c r="J241" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K241" s="10">
         <v>282.05542297417634</v>
       </c>
@@ -17720,9 +18209,14 @@
       <c r="G242" s="7">
         <v>18370</v>
       </c>
-      <c r="H242" s="7"/>
+      <c r="H242" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I242" s="7">
         <v>0</v>
+      </c>
+      <c r="J242" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="K242" s="10">
         <v>0</v>
@@ -17750,10 +18244,15 @@
       <c r="G243" s="7">
         <v>4783</v>
       </c>
-      <c r="H243" s="7"/>
+      <c r="H243" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I243" s="7">
         <v>3916926</v>
       </c>
+      <c r="J243" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K243" s="10">
         <v>818.92661509512857</v>
       </c>
@@ -17780,10 +18279,15 @@
       <c r="G244" s="7">
         <v>17892</v>
       </c>
-      <c r="H244" s="7"/>
+      <c r="H244" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I244" s="7">
         <v>4250202</v>
       </c>
+      <c r="J244" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K244" s="10">
         <v>237.54761904761904</v>
       </c>
@@ -18093,9 +18597,14 @@
       <c r="H253" s="7">
         <v>0</v>
       </c>
-      <c r="I253" s="7"/>
+      <c r="I253" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="J253" s="10">
         <v>0</v>
+      </c>
+      <c r="K253" s="10" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="254" spans="1:11" x14ac:dyDescent="0.25">
@@ -18155,8 +18664,18 @@
       <c r="G255" s="7">
         <v>2314</v>
       </c>
-      <c r="H255" s="7"/>
-      <c r="I255" s="7"/>
+      <c r="H255" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="I255" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="J255" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="K255" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="256" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
@@ -18215,9 +18734,14 @@
       <c r="G257" s="7">
         <v>24625</v>
       </c>
-      <c r="H257" s="7"/>
+      <c r="H257" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I257" s="7">
         <v>0</v>
+      </c>
+      <c r="J257" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="K257" s="10">
         <v>0</v>
@@ -18405,8 +18929,14 @@
       <c r="G263" s="10">
         <v>16209</v>
       </c>
+      <c r="H263" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I263" s="10">
         <v>0</v>
+      </c>
+      <c r="J263" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="K263" s="10">
         <v>0</v>
@@ -18469,9 +18999,15 @@
       <c r="G265" s="10">
         <v>13552</v>
       </c>
+      <c r="H265" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I265" s="10">
         <v>5870625</v>
       </c>
+      <c r="J265" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K265" s="10">
         <v>433.19251770956316</v>
       </c>
@@ -18638,9 +19174,15 @@
       <c r="G270" s="10">
         <v>19850</v>
       </c>
+      <c r="H270" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I270" s="10">
         <v>3954426</v>
       </c>
+      <c r="J270" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K270" s="10">
         <v>199.21541561712846</v>
       </c>
@@ -19090,9 +19632,15 @@
       <c r="H283" s="10">
         <v>62537292</v>
       </c>
+      <c r="I283" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="J283" s="10">
         <v>87.745283521861509</v>
       </c>
+      <c r="K283" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="284" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A284" s="6" t="s">
@@ -19186,9 +19734,15 @@
       <c r="G286" s="10">
         <v>6020</v>
       </c>
+      <c r="H286" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I286" s="10">
         <v>1747487</v>
       </c>
+      <c r="J286" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K286" s="10">
         <v>290.28023255813952</v>
       </c>
@@ -19215,9 +19769,15 @@
       <c r="G287" s="10">
         <v>15454</v>
       </c>
+      <c r="H287" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I287" s="10">
         <v>3226661</v>
       </c>
+      <c r="J287" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K287" s="10">
         <v>208.7913161640999</v>
       </c>
@@ -19244,9 +19804,15 @@
       <c r="G288" s="10">
         <v>17048</v>
       </c>
+      <c r="H288" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I288" s="10">
         <v>4594380</v>
       </c>
+      <c r="J288" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K288" s="10">
         <v>269.4967151572032</v>
       </c>
@@ -19311,8 +19877,14 @@
       <c r="H290" s="10">
         <v>0</v>
       </c>
+      <c r="I290" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="J290" s="10">
         <v>0</v>
+      </c>
+      <c r="K290" s="10" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="291" spans="1:11" x14ac:dyDescent="0.25">
@@ -19687,9 +20259,15 @@
       <c r="G301" s="10">
         <v>153328</v>
       </c>
+      <c r="H301" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I301" s="10">
         <v>11939137</v>
       </c>
+      <c r="J301" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K301" s="10">
         <v>77.866645361577795</v>
       </c>
@@ -19751,6 +20329,18 @@
       <c r="G303" s="10">
         <v>13124</v>
       </c>
+      <c r="H303" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="I303" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="J303" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="K303" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="304" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A304" s="6" t="s">
@@ -19809,8 +20399,14 @@
       <c r="G305" s="10">
         <v>42305</v>
       </c>
+      <c r="H305" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I305" s="10">
         <v>0</v>
+      </c>
+      <c r="J305" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="K305" s="10">
         <v>0</v>
@@ -19838,9 +20434,15 @@
       <c r="G306" s="10">
         <v>28306</v>
       </c>
+      <c r="H306" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I306" s="10">
         <v>6964224</v>
       </c>
+      <c r="J306" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K306" s="10">
         <v>246.03349113262206</v>
       </c>
@@ -19867,6 +20469,18 @@
       <c r="G307" s="10">
         <v>18362</v>
       </c>
+      <c r="H307" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="I307" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="J307" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="K307" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="308" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A308" s="6" t="s">
@@ -19890,9 +20504,15 @@
       <c r="G308" s="10">
         <v>4843</v>
       </c>
+      <c r="H308" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I308" s="10">
         <v>3613206</v>
       </c>
+      <c r="J308" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K308" s="10">
         <v>746.06772661573405</v>
       </c>
@@ -19919,9 +20539,15 @@
       <c r="G309" s="10">
         <v>18151</v>
       </c>
+      <c r="H309" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I309" s="10">
         <v>3065794</v>
       </c>
+      <c r="J309" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K309" s="10">
         <v>168.90496391383394</v>
       </c>
@@ -20231,8 +20857,14 @@
       <c r="H318" s="10">
         <v>0</v>
       </c>
+      <c r="I318" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="J318" s="10">
         <v>0</v>
+      </c>
+      <c r="K318" s="10" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="319" spans="1:11" x14ac:dyDescent="0.25">
@@ -20257,9 +20889,15 @@
       <c r="G319" s="10">
         <v>8173</v>
       </c>
+      <c r="H319" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="I319" s="10">
         <v>3366468</v>
       </c>
+      <c r="J319" s="10" t="s">
+        <v>148</v>
+      </c>
       <c r="K319" s="10">
         <v>411.90113789306253</v>
       </c>
@@ -20286,6 +20924,18 @@
       <c r="G320" s="10">
         <v>2301</v>
       </c>
+      <c r="H320" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="I320" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="J320" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="K320" s="10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="321" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A321" s="6" t="s">
@@ -20480,7 +21130,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K326" xr:uid="{FA323755-867C-4778-921B-8AE7EF507F1F}"/>
+  <autoFilter ref="A1:K1" xr:uid="{82E4BF26-CEE8-4A7D-A75D-E40571B274F8}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>